<commit_message>
replace with correct files
</commit_message>
<xml_diff>
--- a/testdata/excel2json/new_excel2json_files/test-name (test_label)/properties.xlsx
+++ b/testdata/excel2json/new_excel2json_files/test-name (test_label)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F11C06C-D0B1-1A41-B8C7-8754B0C740B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C87B451-B67A-8B45-B9E0-233654C83063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="36880" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="145">
   <si>
     <t>name</t>
   </si>
@@ -353,24 +353,6 @@
   </si>
   <si>
     <t>TimeStamp</t>
-  </si>
-  <si>
-    <t>hasInterval</t>
-  </si>
-  <si>
-    <t>Time interval</t>
-  </si>
-  <si>
-    <t>Zeitintervall</t>
-  </si>
-  <si>
-    <t>hasSequenceBounds</t>
-  </si>
-  <si>
-    <t>IntervalValue</t>
-  </si>
-  <si>
-    <t>Interval</t>
   </si>
   <si>
     <t>hasBoolean</t>
@@ -883,11 +865,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -947,7 +929,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -1074,7 +1056,7 @@
         <v>43</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>44</v>
@@ -1243,7 +1225,7 @@
         <v>65</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>66</v>
@@ -1577,144 +1559,135 @@
         <v>113</v>
       </c>
       <c r="L17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="G18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="G19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="O19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" t="s">
         <v>126</v>
       </c>
-      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" t="s">
         <v>127</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="5"/>
+      <c r="L20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" t="s">
         <v>129</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="L20" s="4" t="s">
+      <c r="O20" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="M20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="N20" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="O20" s="4" t="s">
+      <c r="B21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="L21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" t="s">
-        <v>135</v>
-      </c>
-      <c r="O21" t="s">
-        <v>24</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
       <c r="L22" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4" t="s">
@@ -1723,17 +1696,17 @@
     </row>
     <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C23" s="5"/>
       <c r="L23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4" t="s">
@@ -1742,17 +1715,20 @@
     </row>
     <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C24" s="5"/>
+      <c r="J24" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="L24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="s">
@@ -1761,20 +1737,20 @@
     </row>
     <row r="25" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="J25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>26</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
@@ -1783,42 +1759,20 @@
     </row>
     <row r="26" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="I26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4" t="s">
-        <v>24</v>
+      <c r="C26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>